<commit_message>
multiprocessing now works for grid searches
</commit_message>
<xml_diff>
--- a/resources/data/test_data2.xlsx
+++ b/resources/data/test_data2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\masters\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5BEAD034-ACFB-4755-B73C-ADC2C9E81554}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE10FFFD-AD12-4338-863A-7087517B6F19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{E4F7D1A3-75DE-43FA-ACF2-7CA5E5E65190}"/>
+    <workbookView xWindow="5685" yWindow="2895" windowWidth="38700" windowHeight="15435" xr2:uid="{E4F7D1A3-75DE-43FA-ACF2-7CA5E5E65190}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -416,7 +416,7 @@
   <dimension ref="B1:F458"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="B1" sqref="B1:F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,536 +850,1296 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="1"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="B26" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.78471064814814817</v>
+      </c>
+      <c r="D26" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E26" s="3">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="1"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="B27" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0.78465277777777775</v>
+      </c>
+      <c r="D27" s="3">
+        <v>4.9850000000000003</v>
+      </c>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="1"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
+      <c r="B28" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.78396990740740735</v>
+      </c>
+      <c r="D28" s="3">
+        <v>4.9850000000000003</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="1"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
+      <c r="B29" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.78379629629629621</v>
+      </c>
+      <c r="D29" s="3">
+        <v>4.9850000000000003</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
+      <c r="B30" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.78361111111111104</v>
+      </c>
+      <c r="D30" s="3">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="E30" s="3">
+        <v>5</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="1"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="3"/>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
+      <c r="B31" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.78297453703703701</v>
+      </c>
+      <c r="D31" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E31" s="3">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="1"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="3"/>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
+      <c r="B32" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.7819328703703704</v>
+      </c>
+      <c r="D32" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="1"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="B33" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.781712962962963</v>
+      </c>
+      <c r="D33" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B34" s="1"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="B34" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.78123842592592585</v>
+      </c>
+      <c r="D34" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E34" s="3">
+        <v>1</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="1"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+      <c r="B35" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.78118055555555566</v>
+      </c>
+      <c r="D35" s="3">
+        <v>4.984</v>
+      </c>
+      <c r="E35" s="3">
+        <v>1</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="1"/>
-      <c r="C36" s="2"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+      <c r="B36" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.780787037037037</v>
+      </c>
+      <c r="D36" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="1"/>
-      <c r="C37" s="2"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
+      <c r="B37" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.78008101851851863</v>
+      </c>
+      <c r="D37" s="3">
+        <v>4.9820000000000002</v>
+      </c>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="1"/>
-      <c r="C38" s="2"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
+      <c r="B38" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.77983796296296293</v>
+      </c>
+      <c r="D38" s="3">
+        <v>4.984</v>
+      </c>
+      <c r="E38" s="3">
+        <v>1</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="1"/>
-      <c r="C39" s="2"/>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
+      <c r="B39" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.77938657407407408</v>
+      </c>
+      <c r="D39" s="3">
+        <v>4.984</v>
+      </c>
+      <c r="E39" s="3">
+        <v>2</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="1"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="3"/>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
+      <c r="B40" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.77915509259259252</v>
+      </c>
+      <c r="D40" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E40" s="3">
+        <v>1</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="1"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
+      <c r="B41" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.77913194444444445</v>
+      </c>
+      <c r="D41" s="3">
+        <v>4.984</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="1"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
+      <c r="B42" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.7785185185185185</v>
+      </c>
+      <c r="D42" s="3">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="1"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
+      <c r="B43" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.77798611111111116</v>
+      </c>
+      <c r="D43" s="3">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="1"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
+      <c r="B44" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.77792824074074074</v>
+      </c>
+      <c r="D44" s="3">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="1"/>
-      <c r="C45" s="2"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="B45" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.77789351851851851</v>
+      </c>
+      <c r="D45" s="3">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="46" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="1"/>
-      <c r="C46" s="2"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="B46" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.7777546296296296</v>
+      </c>
+      <c r="D46" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="1"/>
-      <c r="C47" s="2"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="B47" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.7775347222222222</v>
+      </c>
+      <c r="D47" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="1"/>
-      <c r="C48" s="2"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
+      <c r="B48" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.77696759259259263</v>
+      </c>
+      <c r="D48" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="1"/>
-      <c r="C49" s="2"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
+      <c r="B49" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.77695601851851848</v>
+      </c>
+      <c r="D49" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="1"/>
-      <c r="C50" s="2"/>
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
+      <c r="B50" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.77637731481481476</v>
+      </c>
+      <c r="D50" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B51" s="1"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
+      <c r="B51" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C51" s="2">
+        <v>0.77568287037037031</v>
+      </c>
+      <c r="D51" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="52" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B52" s="1"/>
-      <c r="C52" s="2"/>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
+      <c r="B52" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C52" s="2">
+        <v>0.77568287037037031</v>
+      </c>
+      <c r="D52" s="3">
+        <v>4.9740000000000002</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="1"/>
-      <c r="C53" s="2"/>
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
+      <c r="B53" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C53" s="2">
+        <v>0.77545138888888887</v>
+      </c>
+      <c r="D53" s="3">
+        <v>4.9740000000000002</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="54" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="1"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
+      <c r="B54" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C54" s="2">
+        <v>0.77542824074074079</v>
+      </c>
+      <c r="D54" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="1"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+      <c r="B55" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0.77541666666666664</v>
+      </c>
+      <c r="D55" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="56" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B56" s="1"/>
-      <c r="C56" s="2"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
+      <c r="B56" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C56" s="2">
+        <v>0.77541666666666664</v>
+      </c>
+      <c r="D56" s="3">
+        <v>4.9779999999999998</v>
+      </c>
+      <c r="E56" s="3">
+        <v>3</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B57" s="1"/>
-      <c r="C57" s="2"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
+      <c r="B57" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C57" s="2">
+        <v>0.77541666666666664</v>
+      </c>
+      <c r="D57" s="3">
+        <v>4.9779999999999998</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="58" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B58" s="1"/>
-      <c r="C58" s="2"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
+      <c r="B58" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C58" s="2">
+        <v>0.77533564814814815</v>
+      </c>
+      <c r="D58" s="3">
+        <v>4.9820000000000002</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B59" s="1"/>
-      <c r="C59" s="2"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
+      <c r="B59" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C59" s="2">
+        <v>0.77483796296296292</v>
+      </c>
+      <c r="D59" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="60" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="1"/>
-      <c r="C60" s="2"/>
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
+      <c r="B60" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C60" s="2">
+        <v>0.77482638888888899</v>
+      </c>
+      <c r="D60" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B61" s="1"/>
-      <c r="C61" s="2"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
+      <c r="B61" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C61" s="2">
+        <v>0.7747222222222222</v>
+      </c>
+      <c r="D61" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E61" s="3">
+        <v>3</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B62" s="1"/>
-      <c r="C62" s="2"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
+      <c r="B62" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C62" s="2">
+        <v>0.77432870370370377</v>
+      </c>
+      <c r="D62" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B63" s="1"/>
-      <c r="C63" s="2"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
+      <c r="B63" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C63" s="2">
+        <v>0.77429398148148154</v>
+      </c>
+      <c r="D63" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E63" s="3">
+        <v>1</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="64" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B64" s="1"/>
-      <c r="C64" s="2"/>
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
+      <c r="B64" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C64" s="2">
+        <v>0.77302083333333327</v>
+      </c>
+      <c r="D64" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E64" s="3">
+        <v>1</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B65" s="1"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
+      <c r="B65" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C65" s="2">
+        <v>0.77293981481481477</v>
+      </c>
+      <c r="D65" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E65" s="3">
+        <v>1</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="66" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B66" s="1"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
+      <c r="B66" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C66" s="2">
+        <v>0.77293981481481477</v>
+      </c>
+      <c r="D66" s="3">
+        <v>4.9820000000000002</v>
+      </c>
+      <c r="E66" s="3">
+        <v>1</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="67" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B67" s="1"/>
-      <c r="C67" s="2"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
+      <c r="B67" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C67" s="2">
+        <v>0.7726736111111111</v>
+      </c>
+      <c r="D67" s="3">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="E67" s="3">
+        <v>1</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="68" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B68" s="1"/>
-      <c r="C68" s="2"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
+      <c r="B68" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C68" s="2">
+        <v>0.77229166666666671</v>
+      </c>
+      <c r="D68" s="3">
+        <v>4.9829999999999997</v>
+      </c>
+      <c r="E68" s="3">
+        <v>1</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="69" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B69" s="1"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
+      <c r="B69" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C69" s="2">
+        <v>0.77217592592592599</v>
+      </c>
+      <c r="D69" s="3">
+        <v>4.9820000000000002</v>
+      </c>
+      <c r="E69" s="3">
+        <v>2</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="70" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B70" s="1"/>
-      <c r="C70" s="2"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
+      <c r="B70" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C70" s="2">
+        <v>0.77186342592592594</v>
+      </c>
+      <c r="D70" s="3">
+        <v>4.9809999999999999</v>
+      </c>
+      <c r="E70" s="3">
+        <v>1</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="71" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B71" s="1"/>
-      <c r="C71" s="2"/>
-      <c r="D71" s="3"/>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
+      <c r="B71" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0.77164351851851853</v>
+      </c>
+      <c r="D71" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E71" s="3">
+        <v>3</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="72" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B72" s="1"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="3"/>
-      <c r="E72" s="3"/>
-      <c r="F72" s="3"/>
+      <c r="B72" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0.77164351851851853</v>
+      </c>
+      <c r="D72" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E72" s="3">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="73" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B73" s="1"/>
-      <c r="C73" s="2"/>
-      <c r="D73" s="3"/>
-      <c r="E73" s="3"/>
-      <c r="F73" s="3"/>
+      <c r="B73" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C73" s="2">
+        <v>0.77144675925925921</v>
+      </c>
+      <c r="D73" s="3">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="E73" s="3">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="74" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B74" s="1"/>
-      <c r="C74" s="2"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="3"/>
+      <c r="B74" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C74" s="2">
+        <v>0.77127314814814818</v>
+      </c>
+      <c r="D74" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E74" s="3">
+        <v>2</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="75" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B75" s="1"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="3"/>
-      <c r="E75" s="3"/>
-      <c r="F75" s="3"/>
+      <c r="B75" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C75" s="2">
+        <v>0.77087962962962964</v>
+      </c>
+      <c r="D75" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E75" s="3">
+        <v>2</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="76" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B76" s="1"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="3"/>
-      <c r="E76" s="3"/>
-      <c r="F76" s="3"/>
+      <c r="B76" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C76" s="2">
+        <v>0.77086805555555549</v>
+      </c>
+      <c r="D76" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E76" s="3">
+        <v>3</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="77" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B77" s="1"/>
-      <c r="C77" s="2"/>
-      <c r="D77" s="3"/>
-      <c r="E77" s="3"/>
-      <c r="F77" s="3"/>
+      <c r="B77" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C77" s="2">
+        <v>0.77008101851851851</v>
+      </c>
+      <c r="D77" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E77" s="3">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="78" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B78" s="1"/>
-      <c r="C78" s="2"/>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
+      <c r="B78" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C78" s="2">
+        <v>0.77005787037037043</v>
+      </c>
+      <c r="D78" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E78" s="3">
+        <v>3</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="79" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B79" s="1"/>
-      <c r="C79" s="2"/>
-      <c r="D79" s="3"/>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
+      <c r="B79" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C79" s="2">
+        <v>0.76995370370370375</v>
+      </c>
+      <c r="D79" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E79" s="3">
+        <v>2</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="80" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B80" s="1"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="3"/>
-      <c r="E80" s="3"/>
-      <c r="F80" s="3"/>
+      <c r="B80" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C80" s="2">
+        <v>0.76995370370370375</v>
+      </c>
+      <c r="D80" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E80" s="3">
+        <v>1</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="81" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B81" s="1"/>
-      <c r="C81" s="2"/>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-      <c r="F81" s="3"/>
+      <c r="B81" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C81" s="2">
+        <v>0.76861111111111102</v>
+      </c>
+      <c r="D81" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E81" s="3">
+        <v>2</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="82" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B82" s="1"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="3"/>
-      <c r="E82" s="3"/>
-      <c r="F82" s="3"/>
+      <c r="B82" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C82" s="2">
+        <v>0.76848379629629626</v>
+      </c>
+      <c r="D82" s="3">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="E82" s="3">
+        <v>1</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="83" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B83" s="1"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="3"/>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3"/>
+      <c r="B83" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C83" s="2">
+        <v>0.76806712962962964</v>
+      </c>
+      <c r="D83" s="3">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="E83" s="3">
+        <v>1</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="84" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B84" s="1"/>
-      <c r="C84" s="2"/>
-      <c r="D84" s="3"/>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3"/>
+      <c r="B84" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C84" s="2">
+        <v>0.76804398148148145</v>
+      </c>
+      <c r="D84" s="3">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="E84" s="3">
+        <v>1</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="85" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B85" s="1"/>
-      <c r="C85" s="2"/>
-      <c r="D85" s="3"/>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3"/>
+      <c r="B85" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C85" s="2">
+        <v>0.76774305555555555</v>
+      </c>
+      <c r="D85" s="3">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="E85" s="3">
+        <v>1</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="86" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B86" s="1"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="3"/>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3"/>
+      <c r="B86" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C86" s="2">
+        <v>0.76760416666666664</v>
+      </c>
+      <c r="D86" s="3">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="E86" s="3">
+        <v>1</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="87" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B87" s="1"/>
-      <c r="C87" s="2"/>
-      <c r="D87" s="3"/>
-      <c r="E87" s="3"/>
-      <c r="F87" s="3"/>
+      <c r="B87" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C87" s="2">
+        <v>0.76759259259259249</v>
+      </c>
+      <c r="D87" s="3">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="E87" s="3">
+        <v>1</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="88" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="1"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="3"/>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3"/>
+      <c r="B88" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C88" s="2">
+        <v>0.76759259259259249</v>
+      </c>
+      <c r="D88" s="3">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="E88" s="3">
+        <v>1</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="89" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="1"/>
-      <c r="C89" s="2"/>
-      <c r="D89" s="3"/>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3"/>
+      <c r="B89" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C89" s="2">
+        <v>0.76759259259259249</v>
+      </c>
+      <c r="D89" s="3">
+        <v>4.9729999999999999</v>
+      </c>
+      <c r="E89" s="3">
+        <v>1</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="90" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="1"/>
-      <c r="C90" s="2"/>
-      <c r="D90" s="3"/>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3"/>
+      <c r="B90" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C90" s="2">
+        <v>0.76759259259259249</v>
+      </c>
+      <c r="D90" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E90" s="3">
+        <v>1</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="91" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="1"/>
-      <c r="C91" s="2"/>
-      <c r="D91" s="3"/>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3"/>
+      <c r="B91" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C91" s="2">
+        <v>0.76759259259259249</v>
+      </c>
+      <c r="D91" s="3">
+        <v>4.9749999999999996</v>
+      </c>
+      <c r="E91" s="3">
+        <v>2</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="92" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="1"/>
-      <c r="C92" s="2"/>
-      <c r="D92" s="3"/>
-      <c r="E92" s="3"/>
-      <c r="F92" s="3"/>
+      <c r="B92" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C92" s="2">
+        <v>0.76758101851851857</v>
+      </c>
+      <c r="D92" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E92" s="3">
+        <v>3</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="93" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="1"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="3"/>
-      <c r="E93" s="3"/>
-      <c r="F93" s="3"/>
+      <c r="B93" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C93" s="2">
+        <v>0.76731481481481489</v>
+      </c>
+      <c r="D93" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E93" s="3">
+        <v>1</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="94" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="1"/>
-      <c r="C94" s="2"/>
-      <c r="D94" s="3"/>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3"/>
+      <c r="B94" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C94" s="2">
+        <v>0.76729166666666659</v>
+      </c>
+      <c r="D94" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E94" s="3">
+        <v>4</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="95" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="1"/>
-      <c r="C95" s="2"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
+      <c r="B95" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C95" s="2">
+        <v>0.76714120370370376</v>
+      </c>
+      <c r="D95" s="3">
+        <v>4.976</v>
+      </c>
+      <c r="E95" s="3">
+        <v>1</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="96" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="1"/>
-      <c r="C96" s="2"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
+      <c r="B96" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C96" s="2">
+        <v>0.76695601851851858</v>
+      </c>
+      <c r="D96" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E96" s="3">
+        <v>1</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="97" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B97" s="1"/>
-      <c r="C97" s="2"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
+      <c r="B97" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C97" s="2">
+        <v>0.76688657407407401</v>
+      </c>
+      <c r="D97" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E97" s="3">
+        <v>1</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="98" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B98" s="1"/>
-      <c r="C98" s="2"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
+      <c r="B98" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C98" s="2">
+        <v>0.76677083333333329</v>
+      </c>
+      <c r="D98" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E98" s="3">
+        <v>2</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="99" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B99" s="1"/>
-      <c r="C99" s="2"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
+      <c r="B99" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C99" s="2">
+        <v>0.76675925925925925</v>
+      </c>
+      <c r="D99" s="3">
+        <v>4.9770000000000003</v>
+      </c>
+      <c r="E99" s="3">
+        <v>1</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="100" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B100" s="1"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
+      <c r="B100" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C100" s="2">
+        <v>0.76674768518518521</v>
+      </c>
+      <c r="D100" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E100" s="3">
+        <v>1</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="101" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B101" s="1"/>
-      <c r="C101" s="2"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
+      <c r="B101" s="1">
+        <v>44488</v>
+      </c>
+      <c r="C101" s="2">
+        <v>0.76666666666666661</v>
+      </c>
+      <c r="D101" s="3">
+        <v>4.9790000000000001</v>
+      </c>
+      <c r="E101" s="3">
+        <v>1</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="102" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B102" s="1"/>

</xml_diff>